<commit_message>
update prompt expert and summary, template_checklist
</commit_message>
<xml_diff>
--- a/temp/template_checklist_v1.xlsx
+++ b/temp/template_checklist_v1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitlab\ai-proposal\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TuTDA\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F51C796-C223-4F61-AFC9-BF94F4840D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9505DD9-705F-4FC3-990D-2C72DB52DDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>STT</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>Tên gói thầu/ dự án:</t>
-  </si>
-  <si>
-    <t>Link</t>
   </si>
   <si>
     <t>Ngày phát hành</t>
@@ -180,6 +177,12 @@
   </si>
   <si>
     <t>closing_time</t>
+  </si>
+  <si>
+    <t>Giải thích</t>
+  </si>
+  <si>
+    <t>Tham chiếu</t>
   </si>
 </sst>
 </file>
@@ -247,7 +250,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -307,11 +310,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -376,6 +405,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -396,6 +428,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -701,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -712,159 +759,172 @@
     <col min="1" max="1" width="4.81640625" customWidth="1"/>
     <col min="2" max="2" width="28.453125" customWidth="1"/>
     <col min="3" max="3" width="53.6328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" style="2" customWidth="1"/>
-    <col min="6" max="7" width="19.08984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="19.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.08984375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.36328125" style="2" customWidth="1"/>
+    <col min="7" max="8" width="19.08984375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="19.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-    </row>
-    <row r="2" spans="1:8" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="27" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+    </row>
+    <row r="2" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-    </row>
-    <row r="3" spans="1:8" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="28" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+    </row>
+    <row r="3" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="22" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="6" t="s">
+    <row r="5" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="6" t="s">
+    <row r="6" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="28" t="s">
+    <row r="7" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="6" t="s">
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="28" t="s">
+    <row r="8" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="6" t="s">
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="22" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="24" t="s">
+    <row r="9" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="25" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
+      <c r="H9" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-    </row>
-    <row r="11" spans="1:8" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="26"/>
+    </row>
+    <row r="11" spans="1:9" ht="37" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>1</v>
       </c>
@@ -872,7 +932,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>7</v>
@@ -882,9 +942,10 @@
         <v>6</v>
       </c>
       <c r="G11" s="10"/>
-      <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H11" s="10"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>2</v>
       </c>
@@ -900,9 +961,10 @@
         <v>5</v>
       </c>
       <c r="G12" s="10"/>
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H12" s="10"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>3</v>
       </c>
@@ -918,9 +980,10 @@
         <v>5</v>
       </c>
       <c r="G13" s="10"/>
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H13" s="10"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>4</v>
       </c>
@@ -936,9 +999,10 @@
         <v>5</v>
       </c>
       <c r="G14" s="10"/>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="1:8" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H14" s="10"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>5</v>
       </c>
@@ -954,9 +1018,10 @@
         <v>5</v>
       </c>
       <c r="G15" s="10"/>
-      <c r="H15" s="19"/>
-    </row>
-    <row r="16" spans="1:8" ht="122.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H15" s="10"/>
+      <c r="I15" s="19"/>
+    </row>
+    <row r="16" spans="1:9" ht="122.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>6</v>
       </c>
@@ -972,9 +1037,10 @@
         <v>5</v>
       </c>
       <c r="G16" s="10"/>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H16" s="10"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>7</v>
       </c>
@@ -986,23 +1052,25 @@
       <c r="E17" s="7"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="9"/>
-    </row>
-    <row r="18" spans="1:8" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H17" s="10"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>8</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="7"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="9"/>
-    </row>
-    <row r="19" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H18" s="10"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>9</v>
       </c>
@@ -1014,9 +1082,10 @@
       <c r="E19" s="10"/>
       <c r="F19" s="15"/>
       <c r="G19" s="19"/>
-      <c r="H19" s="23"/>
-    </row>
-    <row r="20" spans="1:8" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H19" s="19"/>
+      <c r="I19" s="23"/>
+    </row>
+    <row r="20" spans="1:9" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>10</v>
       </c>
@@ -1028,23 +1097,25 @@
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
-      <c r="H20" s="11"/>
-    </row>
-    <row r="21" spans="1:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H20" s="20"/>
+      <c r="I20" s="11"/>
+    </row>
+    <row r="21" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>11</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
-      <c r="H21" s="11"/>
-    </row>
-    <row r="22" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H21" s="20"/>
+      <c r="I21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>12</v>
       </c>
@@ -1060,9 +1131,10 @@
         <v>6</v>
       </c>
       <c r="G22" s="13"/>
-      <c r="H22" s="11"/>
-    </row>
-    <row r="23" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H22" s="13"/>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>13</v>
       </c>
@@ -1078,9 +1150,10 @@
         <v>6</v>
       </c>
       <c r="G23" s="13"/>
-      <c r="H23" s="11"/>
-    </row>
-    <row r="24" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H23" s="13"/>
+      <c r="I23" s="11"/>
+    </row>
+    <row r="24" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>14</v>
       </c>
@@ -1094,25 +1167,27 @@
       <c r="E24" s="8"/>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
-      <c r="H24" s="12"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="H9:H10"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="A7:G7"/>
     <mergeCell ref="A8:G8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="A3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.2" top="0.8" bottom="0.48" header="0.3" footer="0.18"/>
   <pageSetup paperSize="9" scale="84" orientation="landscape" r:id="rId1"/>

</xml_diff>